<commit_message>
Some modifications in makeDoubleVectorString, printVectorDifferenceInfoFromVectors, Logging
</commit_message>
<xml_diff>
--- a/trunk/CUDA/Resources/Wykres_JakoscUczenia.xlsx
+++ b/trunk/CUDA/Resources/Wykres_JakoscUczenia.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="27960" windowHeight="14595" tabRatio="347" activeTab="6"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18750" windowHeight="8220" tabRatio="347" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -3673,25 +3673,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="71099904"/>
-        <c:axId val="71782784"/>
+        <c:axId val="68914176"/>
+        <c:axId val="68928256"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="71099904"/>
+        <c:axId val="68914176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71782784"/>
+        <c:crossAx val="68928256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="71782784"/>
+        <c:axId val="68928256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3699,19 +3699,20 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71099904"/>
+        <c:crossAx val="68914176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4011,25 +4012,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="118070656"/>
-        <c:axId val="118240384"/>
+        <c:axId val="81903616"/>
+        <c:axId val="81905152"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="118070656"/>
+        <c:axId val="81903616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="118240384"/>
+        <c:crossAx val="81905152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="118240384"/>
+        <c:axId val="81905152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4037,20 +4038,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="118070656"/>
+        <c:crossAx val="81903616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4350,25 +4350,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="120408704"/>
-        <c:axId val="120465280"/>
+        <c:axId val="81805312"/>
+        <c:axId val="81806848"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="120408704"/>
+        <c:axId val="81805312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="120465280"/>
+        <c:crossAx val="81806848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="120465280"/>
+        <c:axId val="81806848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4376,20 +4376,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="120408704"/>
+        <c:crossAx val="81805312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4689,25 +4688,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="120459264"/>
-        <c:axId val="120460800"/>
+        <c:axId val="81940480"/>
+        <c:axId val="81942016"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="120459264"/>
+        <c:axId val="81940480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="120460800"/>
+        <c:crossAx val="81942016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="120460800"/>
+        <c:axId val="81942016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4715,20 +4714,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="120459264"/>
+        <c:crossAx val="81940480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5023,25 +5021,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="128043264"/>
-        <c:axId val="127520768"/>
+        <c:axId val="82026880"/>
+        <c:axId val="82028416"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="128043264"/>
+        <c:axId val="82026880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="127520768"/>
+        <c:crossAx val="82028416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="127520768"/>
+        <c:axId val="82028416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5049,7 +5047,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="128043264"/>
+        <c:crossAx val="82026880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5062,7 +5060,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5357,25 +5355,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="127154432"/>
-        <c:axId val="127168512"/>
+        <c:axId val="82129280"/>
+        <c:axId val="82130816"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="127154432"/>
+        <c:axId val="82129280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="127168512"/>
+        <c:crossAx val="82130816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="127168512"/>
+        <c:axId val="82130816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5383,7 +5381,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="127154432"/>
+        <c:crossAx val="82129280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5396,7 +5394,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5691,25 +5689,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="128059648"/>
-        <c:axId val="128069632"/>
+        <c:axId val="82170240"/>
+        <c:axId val="82171776"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="128059648"/>
+        <c:axId val="82170240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="128069632"/>
+        <c:crossAx val="82171776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="128069632"/>
+        <c:axId val="82171776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5717,20 +5715,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="128059648"/>
+        <c:crossAx val="82170240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5865,25 +5862,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="75190272"/>
-        <c:axId val="75229440"/>
+        <c:axId val="78145024"/>
+        <c:axId val="78146560"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="75190272"/>
+        <c:axId val="78145024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75229440"/>
+        <c:crossAx val="78146560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="75229440"/>
+        <c:axId val="78146560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5891,19 +5888,20 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75190272"/>
+        <c:crossAx val="78145024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -6038,25 +6036,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="109732608"/>
-        <c:axId val="109734144"/>
+        <c:axId val="78176256"/>
+        <c:axId val="78177792"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="109732608"/>
+        <c:axId val="78176256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109734144"/>
+        <c:crossAx val="78177792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="109734144"/>
+        <c:axId val="78177792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6064,19 +6062,20 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109732608"/>
+        <c:crossAx val="78176256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -6211,25 +6210,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="109941120"/>
-        <c:axId val="109942656"/>
+        <c:axId val="78248576"/>
+        <c:axId val="78258560"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="109941120"/>
+        <c:axId val="78248576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109942656"/>
+        <c:crossAx val="78258560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="109942656"/>
+        <c:axId val="78258560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6237,7 +6236,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109941120"/>
+        <c:crossAx val="78248576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6249,7 +6248,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -6330,25 +6329,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="111876736"/>
-        <c:axId val="111908352"/>
+        <c:axId val="78288000"/>
+        <c:axId val="78289536"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="111876736"/>
+        <c:axId val="78288000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="111908352"/>
+        <c:crossAx val="78289536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="111908352"/>
+        <c:axId val="78289536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6356,7 +6355,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="111876736"/>
+        <c:crossAx val="78288000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6368,7 +6367,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -6449,25 +6448,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="121659392"/>
-        <c:axId val="121660928"/>
+        <c:axId val="78314880"/>
+        <c:axId val="78324864"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="121659392"/>
+        <c:axId val="78314880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="121660928"/>
+        <c:crossAx val="78324864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="121660928"/>
+        <c:axId val="78324864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6475,7 +6474,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="121659392"/>
+        <c:crossAx val="78314880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6487,7 +6486,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -6787,25 +6786,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="71064576"/>
-        <c:axId val="71111424"/>
+        <c:axId val="80645504"/>
+        <c:axId val="80655488"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="71064576"/>
+        <c:axId val="80645504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71111424"/>
+        <c:crossAx val="80655488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="71111424"/>
+        <c:axId val="80655488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6813,20 +6812,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71064576"/>
+        <c:crossAx val="80645504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -7126,25 +7124,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="76893184"/>
-        <c:axId val="83149568"/>
+        <c:axId val="78400896"/>
+        <c:axId val="78414976"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="76893184"/>
+        <c:axId val="78400896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83149568"/>
+        <c:crossAx val="78414976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="83149568"/>
+        <c:axId val="78414976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7152,20 +7150,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76893184"/>
+        <c:crossAx val="78400896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -7465,25 +7462,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="108944384"/>
-        <c:axId val="108958464"/>
+        <c:axId val="78445952"/>
+        <c:axId val="80692352"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="108944384"/>
+        <c:axId val="78445952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108958464"/>
+        <c:crossAx val="80692352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="108958464"/>
+        <c:axId val="80692352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7491,20 +7488,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108944384"/>
+        <c:crossAx val="78445952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -8272,8 +8268,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="E7:Y91"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12:O18"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -9946,8 +9942,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A5:M22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -16337,8 +16333,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A7:AI187"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="AH16" sqref="AH16"/>
+    <sheetView topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>

</xml_diff>